<commit_message>
i modified ROM into ROU in the nationality column
</commit_message>
<xml_diff>
--- a/dataset_volley.xlsx
+++ b/dataset_volley.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\Final-Crewmates-Project-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF030B5-3D34-4068-8EB8-1E4454824AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DCC1AE-B2FB-439D-A79C-A49477C7AA89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{381DB8E8-216C-41B8-B6DA-A2B4776491B4}"/>
   </bookViews>
@@ -200,9 +200,6 @@
     <t>CYP</t>
   </si>
   <si>
-    <t>ROM</t>
-  </si>
-  <si>
     <t>PIANI VITTORIA</t>
   </si>
   <si>
@@ -705,6 +702,9 @@
   </si>
   <si>
     <t>ZANETTI BERGAMO</t>
+  </si>
+  <si>
+    <t>ROU</t>
   </si>
 </sst>
 </file>
@@ -1222,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772A63F9-E294-419D-A374-792BE1D22AA3}">
   <dimension ref="A1:J183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1237,27 +1237,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>209</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>3</v>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>7</v>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>9</v>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>10</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>12</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>13</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>14</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>15</v>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>17</v>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>18</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>19</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>21</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>22</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="17" spans="1:8" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>23</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>24</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>25</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>26</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>27</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>28</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>29</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>30</v>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>31</v>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>32</v>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>33</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>34</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="29" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B29" s="17" t="s">
         <v>38</v>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="30" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B30" s="17" t="s">
         <v>39</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="31" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>40</v>
@@ -1859,7 +1859,7 @@
     </row>
     <row r="32" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B32" s="17" t="s">
         <v>41</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="33" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>42</v>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="34" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>43</v>
@@ -1925,7 +1925,7 @@
     </row>
     <row r="35" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B35" s="17" t="s">
         <v>44</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="36" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B36" s="17" t="s">
         <v>45</v>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="37" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>46</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="38" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B38" s="17" t="s">
         <v>47</v>
@@ -2013,7 +2013,7 @@
     </row>
     <row r="39" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B39" s="17" t="s">
         <v>48</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="40" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>49</v>
@@ -2050,14 +2050,14 @@
         <v>187</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>55</v>
+        <v>223</v>
       </c>
       <c r="G40" s="23"/>
       <c r="H40" s="23"/>
     </row>
     <row r="41" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B41" s="17" t="s">
         <v>50</v>
@@ -2079,10 +2079,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>20</v>
@@ -2102,10 +2102,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43" s="21" t="s">
         <v>6</v>
@@ -2125,10 +2125,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C44" s="21" t="s">
         <v>6</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" s="21" t="s">
         <v>1</v>
@@ -2171,10 +2171,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>16</v>
@@ -2194,10 +2194,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C47" s="21" t="s">
         <v>4</v>
@@ -2217,10 +2217,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C48" s="21" t="s">
         <v>4</v>
@@ -2240,10 +2240,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49" s="21" t="s">
         <v>6</v>
@@ -2263,10 +2263,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>16</v>
@@ -2286,10 +2286,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51" s="21" t="s">
         <v>16</v>
@@ -2309,10 +2309,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" s="21" t="s">
         <v>6</v>
@@ -2332,10 +2332,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C53" s="21" t="s">
         <v>20</v>
@@ -2355,10 +2355,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C54" s="21" t="s">
         <v>6</v>
@@ -2378,10 +2378,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C55" s="21" t="s">
         <v>6</v>
@@ -2401,10 +2401,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56" s="21" t="s">
         <v>1</v>
@@ -2424,10 +2424,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C57" s="21" t="s">
         <v>20</v>
@@ -2447,10 +2447,10 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58" s="21" t="s">
         <v>4</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59" s="21" t="s">
         <v>6</v>
@@ -2493,10 +2493,10 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C60" s="21" t="s">
         <v>16</v>
@@ -2516,10 +2516,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" s="21" t="s">
         <v>1</v>
@@ -2539,10 +2539,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C62" s="21" t="s">
         <v>4</v>
@@ -2554,7 +2554,7 @@
         <v>180</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G62" s="19"/>
       <c r="H62" s="19"/>
@@ -2562,10 +2562,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C63" s="21" t="s">
         <v>16</v>
@@ -2585,10 +2585,10 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C64" s="21" t="s">
         <v>16</v>
@@ -2600,7 +2600,7 @@
         <v>192</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G64" s="19"/>
       <c r="H64" s="19"/>
@@ -2608,10 +2608,10 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C65" s="21" t="s">
         <v>20</v>
@@ -2623,15 +2623,15 @@
         <v>191</v>
       </c>
       <c r="F65" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C66" s="21" t="s">
         <v>6</v>
@@ -2648,10 +2648,10 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C67" s="21" t="s">
         <v>6</v>
@@ -2672,10 +2672,10 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C68" s="21" t="s">
         <v>6</v>
@@ -2696,10 +2696,10 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C69" s="21" t="s">
         <v>4</v>
@@ -2720,10 +2720,10 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C70" s="21" t="s">
         <v>6</v>
@@ -2735,7 +2735,7 @@
         <v>187</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -2744,10 +2744,10 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C71" s="21" t="s">
         <v>6</v>
@@ -2768,10 +2768,10 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C72" s="21" t="s">
         <v>16</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C73" s="21" t="s">
         <v>1</v>
@@ -2816,10 +2816,10 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C74" s="21" t="s">
         <v>4</v>
@@ -2831,7 +2831,7 @@
         <v>172</v>
       </c>
       <c r="F74" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
@@ -2840,10 +2840,10 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C75" s="21" t="s">
         <v>16</v>
@@ -2864,10 +2864,10 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C76" s="21" t="s">
         <v>6</v>
@@ -2888,10 +2888,10 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" s="21" t="s">
         <v>16</v>
@@ -2912,10 +2912,10 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C78" s="21" t="s">
         <v>20</v>
@@ -2936,10 +2936,10 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C79" s="21" t="s">
         <v>16</v>
@@ -2960,10 +2960,10 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C80" s="21" t="s">
         <v>1</v>
@@ -2984,10 +2984,10 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C81" s="26" t="s">
         <v>1</v>
@@ -3008,10 +3008,10 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82" s="26" t="s">
         <v>20</v>
@@ -3023,7 +3023,7 @@
         <v>189</v>
       </c>
       <c r="F82" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G82" s="19"/>
       <c r="H82" s="2"/>
@@ -3032,10 +3032,10 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C83" s="26" t="s">
         <v>16</v>
@@ -3053,10 +3053,10 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C84" s="26" t="s">
         <v>16</v>
@@ -3074,10 +3074,10 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C85" s="26" t="s">
         <v>16</v>
@@ -3095,10 +3095,10 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C86" s="26" t="s">
         <v>6</v>
@@ -3116,10 +3116,10 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C87" s="26" t="s">
         <v>1</v>
@@ -3137,10 +3137,10 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C88" s="26" t="s">
         <v>6</v>
@@ -3152,16 +3152,16 @@
         <v>192</v>
       </c>
       <c r="F88" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G88" s="19"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C89" s="26" t="s">
         <v>4</v>
@@ -3179,10 +3179,10 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C90" s="26" t="s">
         <v>4</v>
@@ -3194,16 +3194,16 @@
         <v>181</v>
       </c>
       <c r="F90" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G90" s="19"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C91" s="26" t="s">
         <v>6</v>
@@ -3215,16 +3215,16 @@
         <v>193</v>
       </c>
       <c r="F91" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G91" s="19"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C92" s="26" t="s">
         <v>6</v>
@@ -3242,10 +3242,10 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C93" s="26" t="s">
         <v>20</v>
@@ -3263,10 +3263,10 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B94" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C94" s="26" t="s">
         <v>16</v>
@@ -3284,10 +3284,10 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B95" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C95" s="21" t="s">
         <v>16</v>
@@ -3299,17 +3299,17 @@
         <v>195</v>
       </c>
       <c r="F95" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B96" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C96" s="21" t="s">
         <v>6</v>
@@ -3328,10 +3328,10 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C97" s="21" t="s">
         <v>4</v>
@@ -3350,10 +3350,10 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B98" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C98" s="21" t="s">
         <v>6</v>
@@ -3365,17 +3365,17 @@
         <v>185</v>
       </c>
       <c r="F98" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C99" s="21" t="s">
         <v>4</v>
@@ -3387,17 +3387,17 @@
         <v>180</v>
       </c>
       <c r="F99" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B100" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C100" s="21" t="s">
         <v>1</v>
@@ -3416,10 +3416,10 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C101" s="21" t="s">
         <v>20</v>
@@ -3438,10 +3438,10 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B102" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C102" s="21" t="s">
         <v>6</v>
@@ -3460,10 +3460,10 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B103" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C103" s="21" t="s">
         <v>1</v>
@@ -3482,10 +3482,10 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B104" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C104" s="21" t="s">
         <v>20</v>
@@ -3497,17 +3497,17 @@
         <v>188</v>
       </c>
       <c r="F104" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G104" s="19"/>
       <c r="H104" s="19"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B105" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C105" s="21" t="s">
         <v>16</v>
@@ -3526,10 +3526,10 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B106" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C106" s="21" t="s">
         <v>16</v>
@@ -3548,10 +3548,10 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B107" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C107" s="21" t="s">
         <v>6</v>
@@ -3570,10 +3570,10 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B108" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C108" s="21" t="s">
         <v>4</v>
@@ -3594,10 +3594,10 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B109" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C109" s="21" t="s">
         <v>16</v>
@@ -3618,10 +3618,10 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B110" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C110" s="21" t="s">
         <v>16</v>
@@ -3642,10 +3642,10 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B111" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C111" s="21" t="s">
         <v>20</v>
@@ -3666,10 +3666,10 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B112" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C112" s="21" t="s">
         <v>4</v>
@@ -3690,10 +3690,10 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B113" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C113" s="21" t="s">
         <v>6</v>
@@ -3705,7 +3705,7 @@
         <v>185</v>
       </c>
       <c r="F113" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
@@ -3714,10 +3714,10 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B114" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C114" s="21" t="s">
         <v>16</v>
@@ -3738,10 +3738,10 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B115" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C115" s="21" t="s">
         <v>6</v>
@@ -3753,7 +3753,7 @@
         <v>188</v>
       </c>
       <c r="F115" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G115" s="19"/>
       <c r="H115" s="19"/>
@@ -3762,10 +3762,10 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B116" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C116" s="21" t="s">
         <v>6</v>
@@ -3786,10 +3786,10 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B117" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C117" s="21" t="s">
         <v>20</v>
@@ -3810,10 +3810,10 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B118" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C118" s="21" t="s">
         <v>6</v>
@@ -3825,7 +3825,7 @@
         <v>188</v>
       </c>
       <c r="F118" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G118" s="19"/>
       <c r="H118" s="19"/>
@@ -3834,10 +3834,10 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B119" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C119" s="21" t="s">
         <v>1</v>
@@ -3858,10 +3858,10 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B120" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C120" s="21" t="s">
         <v>1</v>
@@ -3882,10 +3882,10 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B121" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C121" s="21" t="s">
         <v>20</v>
@@ -3897,7 +3897,7 @@
         <v>203</v>
       </c>
       <c r="F121" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G121" s="19"/>
       <c r="H121" s="19"/>
@@ -3906,10 +3906,10 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B122" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C122" s="21" t="s">
         <v>4</v>
@@ -3930,10 +3930,10 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B123" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C123" s="21" t="s">
         <v>16</v>
@@ -3954,10 +3954,10 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B124" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C124" s="21" t="s">
         <v>6</v>
@@ -3969,7 +3969,7 @@
         <v>184</v>
       </c>
       <c r="F124" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G124" s="19"/>
       <c r="H124" s="19"/>
@@ -3978,10 +3978,10 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B125" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C125" s="21" t="s">
         <v>6</v>
@@ -4002,10 +4002,10 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B126" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C126" s="21" t="s">
         <v>1</v>
@@ -4026,10 +4026,10 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B127" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C127" s="21" t="s">
         <v>16</v>
@@ -4050,10 +4050,10 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B128" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C128" s="21" t="s">
         <v>1</v>
@@ -4074,10 +4074,10 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B129" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C129" s="21" t="s">
         <v>16</v>
@@ -4098,10 +4098,10 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B130" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C130" s="21" t="s">
         <v>16</v>
@@ -4122,10 +4122,10 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B131" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C131" s="21" t="s">
         <v>20</v>
@@ -4137,7 +4137,7 @@
         <v>188</v>
       </c>
       <c r="F131" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G131" s="19"/>
       <c r="H131" s="19"/>
@@ -4146,10 +4146,10 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B132" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C132" s="21" t="s">
         <v>6</v>
@@ -4170,10 +4170,10 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C133" s="21" t="s">
         <v>6</v>
@@ -4185,7 +4185,7 @@
         <v>185</v>
       </c>
       <c r="F133" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G133" s="19"/>
       <c r="H133" s="19"/>
@@ -4193,10 +4193,10 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B134" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C134" s="21" t="s">
         <v>4</v>
@@ -4216,10 +4216,10 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B135" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C135" s="21" t="s">
         <v>4</v>
@@ -4231,7 +4231,7 @@
         <v>188</v>
       </c>
       <c r="F135" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G135" s="19"/>
       <c r="H135" s="19"/>
@@ -4240,10 +4240,10 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B136" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C136" s="21" t="s">
         <v>16</v>
@@ -4264,10 +4264,10 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B137" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C137" s="21" t="s">
         <v>6</v>
@@ -4288,10 +4288,10 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C138" s="21" t="s">
         <v>4</v>
@@ -4312,10 +4312,10 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B139" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C139" s="21" t="s">
         <v>6</v>
@@ -4327,7 +4327,7 @@
         <v>185</v>
       </c>
       <c r="F139" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G139" s="19"/>
       <c r="H139" s="19"/>
@@ -4336,10 +4336,10 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B140" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C140" s="21" t="s">
         <v>1</v>
@@ -4360,10 +4360,10 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B141" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C141" s="21" t="s">
         <v>20</v>
@@ -4384,10 +4384,10 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B142" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C142" s="21" t="s">
         <v>6</v>
@@ -4408,10 +4408,10 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B143" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C143" s="21" t="s">
         <v>1</v>
@@ -4432,10 +4432,10 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B144" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C144" s="21" t="s">
         <v>16</v>
@@ -4456,10 +4456,10 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B145" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C145" s="21" t="s">
         <v>6</v>
@@ -4471,7 +4471,7 @@
         <v>184</v>
       </c>
       <c r="F145" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G145" s="19"/>
       <c r="H145" s="19"/>
@@ -4480,10 +4480,10 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B146" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C146" s="21" t="s">
         <v>6</v>
@@ -4504,10 +4504,10 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B147" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C147" s="21" t="s">
         <v>16</v>
@@ -4528,10 +4528,10 @@
     </row>
     <row r="148" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B148" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C148" s="21" t="s">
         <v>16</v>
@@ -4552,10 +4552,10 @@
     </row>
     <row r="149" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B149" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C149" s="21" t="s">
         <v>4</v>
@@ -4567,7 +4567,7 @@
         <v>180</v>
       </c>
       <c r="F149" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G149" s="19"/>
       <c r="H149" s="19"/>
@@ -4576,10 +4576,10 @@
     </row>
     <row r="150" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B150" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C150" s="21" t="s">
         <v>6</v>
@@ -4600,10 +4600,10 @@
     </row>
     <row r="151" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B151" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C151" s="21" t="s">
         <v>1</v>
@@ -4624,10 +4624,10 @@
     </row>
     <row r="152" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B152" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C152" s="21" t="s">
         <v>4</v>
@@ -4648,10 +4648,10 @@
     </row>
     <row r="153" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B153" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C153" s="21" t="s">
         <v>20</v>
@@ -4663,7 +4663,7 @@
         <v>186</v>
       </c>
       <c r="F153" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G153" s="19"/>
       <c r="H153" s="19"/>
@@ -4672,10 +4672,10 @@
     </row>
     <row r="154" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B154" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C154" s="21" t="s">
         <v>1</v>
@@ -4696,10 +4696,10 @@
     </row>
     <row r="155" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B155" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C155" s="21" t="s">
         <v>16</v>
@@ -4718,10 +4718,10 @@
     </row>
     <row r="156" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B156" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C156" s="21" t="s">
         <v>20</v>
@@ -4740,10 +4740,10 @@
     </row>
     <row r="157" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B157" s="20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C157" s="21" t="s">
         <v>16</v>
@@ -4762,10 +4762,10 @@
     </row>
     <row r="158" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B158" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C158" s="21" t="s">
         <v>4</v>
@@ -4777,17 +4777,17 @@
         <v>177</v>
       </c>
       <c r="F158" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G158" s="19"/>
       <c r="H158" s="19"/>
     </row>
     <row r="159" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B159" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C159" s="21" t="s">
         <v>6</v>
@@ -4799,17 +4799,17 @@
         <v>198</v>
       </c>
       <c r="F159" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G159" s="19"/>
       <c r="H159" s="19"/>
     </row>
     <row r="160" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B160" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C160" s="21" t="s">
         <v>6</v>
@@ -4821,17 +4821,17 @@
         <v>194</v>
       </c>
       <c r="F160" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G160" s="19"/>
       <c r="H160" s="19"/>
     </row>
     <row r="161" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B161" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C161" s="21" t="s">
         <v>6</v>
@@ -4850,10 +4850,10 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B162" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C162" s="21" t="s">
         <v>6</v>
@@ -4865,17 +4865,17 @@
         <v>190</v>
       </c>
       <c r="F162" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G162" s="19"/>
       <c r="H162" s="19"/>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B163" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C163" s="21" t="s">
         <v>6</v>
@@ -4887,17 +4887,17 @@
         <v>179</v>
       </c>
       <c r="F163" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G163" s="19"/>
       <c r="H163" s="19"/>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B164" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C164" s="21" t="s">
         <v>4</v>
@@ -4916,10 +4916,10 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B165" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C165" s="21" t="s">
         <v>1</v>
@@ -4938,10 +4938,10 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B166" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C166" s="21" t="s">
         <v>6</v>
@@ -4960,10 +4960,10 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B167" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C167" s="21" t="s">
         <v>20</v>
@@ -4982,10 +4982,10 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B168" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C168" s="21" t="s">
         <v>16</v>
@@ -5004,10 +5004,10 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B169" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C169" s="21" t="s">
         <v>4</v>
@@ -5019,17 +5019,17 @@
         <v>170</v>
       </c>
       <c r="F169" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G169" s="19"/>
       <c r="H169" s="19"/>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B170" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C170" s="21" t="s">
         <v>1</v>
@@ -5048,10 +5048,10 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B171" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C171" s="21" t="s">
         <v>6</v>
@@ -5063,17 +5063,17 @@
         <v>186</v>
       </c>
       <c r="F171" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G171" s="19"/>
       <c r="H171" s="19"/>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B172" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C172" s="21" t="s">
         <v>6</v>
@@ -5092,10 +5092,10 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B173" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C173" s="21" t="s">
         <v>16</v>
@@ -5114,10 +5114,10 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B174" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C174" s="21" t="s">
         <v>16</v>

</xml_diff>